<commit_message>
Modified Code in File upload for Primary Secondary
</commit_message>
<xml_diff>
--- a/wwwroot/ExcelSample/ExcelSample.xlsx
+++ b/wwwroot/ExcelSample/ExcelSample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\source\repos\VehicleManagement\wwwroot\ExcelSample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhammadsalman\source\repos\VehicleManagement\wwwroot\ExcelSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,9 +23,90 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>Transaction Date</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Lorry No</t>
+  </si>
+  <si>
+    <t>Vendor Name</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Stock Transfer Advice #</t>
+  </si>
+  <si>
+    <t>Stock Transfer Advice Quantity</t>
+  </si>
+  <si>
+    <t>Supply Point</t>
+  </si>
+  <si>
+    <t>Receipt Point</t>
+  </si>
+  <si>
+    <t>Primary Freight</t>
+  </si>
+  <si>
+    <t>Primary Freight Value</t>
+  </si>
+  <si>
+    <t>Primary Shortage (Ltrs)</t>
+  </si>
+  <si>
+    <t>P-Shortage Charge to Carriage</t>
+  </si>
+  <si>
+    <t>Exemption (Ltrs)</t>
+  </si>
+  <si>
+    <t>Ex Depot Price</t>
+  </si>
+  <si>
+    <t>Value of Primary Shortage</t>
+  </si>
+  <si>
+    <t>Value of Shortage Exempted on Terperature</t>
+  </si>
+  <si>
+    <t>Value of Shortage Charged to Carriage</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>TMG-941</t>
+  </si>
+  <si>
+    <t>SHAKOOR &amp; CO.</t>
+  </si>
+  <si>
+    <t>Petroleum Motor Gasoline - PMG</t>
+  </si>
+  <si>
+    <t>KMR-ZYCO</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +114,63 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,17 +178,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -336,14 +532,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G8" sqref="G7:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>45292</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+      <c r="N2" s="10">
+        <v>0</v>
+      </c>
+      <c r="O2" s="12">
+        <v>0</v>
+      </c>
+      <c r="P2" s="13">
+        <f t="shared" ref="P2" si="0">L2*O2</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>0</v>
+      </c>
+      <c r="R2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F1:F2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>